<commit_message>
Added RUN_ME file to execute .py files more elegantly, and other minor updates
</commit_message>
<xml_diff>
--- a/Fishlist.xlsx
+++ b/Fishlist.xlsx
@@ -438,7 +438,6 @@
           <t>November-March (Northern) / May-September (Southern)</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -472,7 +471,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -506,7 +504,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -540,7 +537,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -574,7 +570,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -608,7 +603,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -642,7 +636,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -676,7 +669,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -710,7 +702,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -744,7 +735,6 @@
           <t>April-August (Northern) / October-February (Southern)</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -778,7 +768,6 @@
           <t>April-September (Northern) / October-March (Southern)</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -812,7 +801,6 @@
           <t>August-September (Northern) / February-March (Southern)</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -846,7 +834,6 @@
           <t>April-October (Northern) / October-April (Southern)</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -880,7 +867,6 @@
           <t>March-July (Northern) / September-January (Southern)</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -914,7 +900,6 @@
           <t>May-August (Northern) / November-Feburary (Southern)</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -948,7 +933,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -982,7 +966,6 @@
           <t>March-May (Northern) / September-November (Southern)</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1016,7 +999,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1050,7 +1032,6 @@
           <t>June-August (Northern) / December-February (Southern)</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1084,7 +1065,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1118,7 +1098,6 @@
           <t>October-March (Northern) / April-September (Southern)</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1152,7 +1131,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1186,7 +1164,6 @@
           <t>June-October (Northern) / December-April (Southern)</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1220,7 +1197,6 @@
           <t>September-December (Northern) / March-June (Southern)</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1254,7 +1230,6 @@
           <t>December-February (Northern) / June-August (Southern)</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1288,7 +1263,6 @@
           <t>July-September (Northern) / January-March (Southern)</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1322,7 +1296,6 @@
           <t>March-June, September-November (Northern) / March-May, September-December (Southern)</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1356,7 +1329,6 @@
           <t>March-June, September-November (Northern) / March-May, September-December (Southern)</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1390,7 +1362,6 @@
           <t>March-June, September-November (Northern) / March-May, September-December (Southern)</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1424,7 +1395,6 @@
           <t>December-March (Northern) / June-September (Southern)</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1458,7 +1428,6 @@
           <t>September (Northern) / March (Southern)</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1492,7 +1461,6 @@
           <t>September (Northern) / March (Southern)</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1526,7 +1494,6 @@
           <t>September-November (Northern) / March-May (Southern)</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1560,7 +1527,6 @@
           <t>April-November (Northern) / October-May (Southern)</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1594,7 +1560,6 @@
           <t>May-September (Northern) / November-March (Southern)</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1628,7 +1593,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1662,7 +1626,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1696,7 +1659,6 @@
           <t>April-November (Northern) / October-May (Southern)</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1730,7 +1692,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1764,7 +1725,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1798,7 +1758,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1832,7 +1791,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1866,7 +1824,6 @@
           <t>July-October (Northern) / January-April (Southern)</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1900,7 +1857,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1934,7 +1890,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1968,7 +1923,6 @@
           <t>September-March (Northern) / March-September (Southern)</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2002,7 +1956,6 @@
           <t>December-March (Northern) / June-September (Southern)</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2036,7 +1989,6 @@
           <t>April-November (Northern) / October-May (Southern)</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2070,7 +2022,6 @@
           <t>April-September (Northern) / October-March (Southern)</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2104,7 +2055,6 @@
           <t>April-September (Northern) / October-March (Southern)</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2138,7 +2088,6 @@
           <t>April-September (Northern) / October-March (Southern)</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2172,7 +2121,6 @@
           <t>July-August (Northern) / January-February (Southern)</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2206,7 +2154,6 @@
           <t>April-November (Northern) / October-May (Southern)</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2240,7 +2187,6 @@
           <t>November-February (Northern) / May-August (Southern)</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2274,7 +2220,6 @@
           <t>July-September (Northern) / January-March (Southern)</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2308,7 +2253,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2342,7 +2286,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2376,7 +2319,6 @@
           <t>March-November (Northern) / September-May (Southern)</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2410,7 +2352,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2444,7 +2385,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2478,7 +2418,6 @@
           <t>October-April (Northern) / April-October (Southern)</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2512,7 +2451,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2546,7 +2484,6 @@
           <t>December-August (Northern) / June-February (Southern)</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2580,7 +2517,6 @@
           <t>August-October (Northern) / February-April (Southern)</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2614,7 +2550,6 @@
           <t>June-October (Northern) / December-April (Southern)</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2648,7 +2583,6 @@
           <t>November-April (Northern) / May-October (Southern)</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2682,7 +2616,6 @@
           <t>July-September, November-April (Northern) / January-March, May-November (Southern)</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2716,7 +2649,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2750,7 +2682,6 @@
           <t>May-October (Northern) / November-April (Southern)</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2784,7 +2715,6 @@
           <t>July-September (Northern) / January-March (Southern)</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2818,7 +2748,6 @@
           <t>August-November (Northern) / February-May (Southern)</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2852,7 +2781,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2886,7 +2814,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2920,7 +2847,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -2954,7 +2880,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2988,7 +2913,6 @@
           <t>June-September (Northern) / December-March (Southern)</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -3022,7 +2946,6 @@
           <t>November-March (Northern) / May-September (Southern)</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -3056,7 +2979,6 @@
           <t>December-May (Northern) / June-November (Southern)</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -3090,7 +3012,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3124,7 +3045,6 @@
           <t>Year-round (Northern and Southern)</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>